<commit_message>
Done Detail Sertifikasi Pelatihan
</commit_message>
<xml_diff>
--- a/public/template_datapengguna - Copy.xlsx
+++ b/public/template_datapengguna - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\siertify\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B9E19D-499C-4C91-9CA1-FCE2721FD508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3392654-086A-4DE7-BFF4-83F6B9F0B143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{63E89108-CD08-4C4E-98FF-9856EE0AFF42}"/>
+    <workbookView xWindow="28455" yWindow="3000" windowWidth="18000" windowHeight="9810" xr2:uid="{63E89108-CD08-4C4E-98FF-9856EE0AFF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,51 +34,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>nama_lengkap</t>
-  </si>
-  <si>
-    <t>NIP</t>
-  </si>
-  <si>
-    <t>tempat_lahir</t>
-  </si>
-  <si>
-    <t>tanggal_lahir</t>
-  </si>
-  <si>
-    <t>jenis_kelamin</t>
-  </si>
-  <si>
-    <t>alamat</t>
-  </si>
-  <si>
-    <t>no_telp</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Topek</t>
-  </si>
-  <si>
-    <t>2241762051</t>
-  </si>
-  <si>
-    <t>Sidoarjo</t>
-  </si>
-  <si>
-    <t>laki</t>
-  </si>
-  <si>
-    <t>Jl. Suhat bro no. 123</t>
-  </si>
-  <si>
-    <t>081515430129</t>
-  </si>
-  <si>
-    <t>topegila@gmail.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ID Pelatihan</t>
+  </si>
+  <si>
+    <t>ID Periode</t>
+  </si>
+  <si>
+    <t>ID User</t>
+  </si>
+  <si>
+    <t>Tanggal Mulai</t>
+  </si>
+  <si>
+    <t>Tanggal Selesai</t>
+  </si>
+  <si>
+    <t>Lokasi</t>
+  </si>
+  <si>
+    <t>Quota Peserta</t>
+  </si>
+  <si>
+    <t>Biaya</t>
+  </si>
+  <si>
+    <t>Input</t>
   </si>
 </sst>
 </file>
@@ -86,9 +71,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +85,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,11 +117,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,16 +440,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB15611-44A7-4330-A265-6388353EDB40}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -464,17 +458,17 @@
     <col min="8" max="8" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -489,37 +483,17 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3">
-        <v>37710</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H2" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{36B81F42-2785-4CA3-811F-E743E7A1FDA7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>